<commit_message>
Moved book 'prueba' from wishlist to biblioteca
</commit_message>
<xml_diff>
--- a/data/nini/Biblioteca.xlsx
+++ b/data/nini/Biblioteca.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C308"/>
+  <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,6 +5593,19 @@
         </is>
       </c>
     </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>prueba</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>actualizada</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new book: Resistencias Lestradas by Ana María Ferreira in Nini's library
</commit_message>
<xml_diff>
--- a/data/nini/Biblioteca.xlsx
+++ b/data/nini/Biblioteca.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C308"/>
+  <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,6 +5593,19 @@
         </is>
       </c>
     </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Resistencias Lestradas</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Ana María Ferreira</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated book: Resistencias Letradas by Ana María Ferreira Hernández in Nini's library
</commit_message>
<xml_diff>
--- a/data/nini/Biblioteca.xlsx
+++ b/data/nini/Biblioteca.xlsx
@@ -5596,15 +5596,19 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Resistencias Lestradas</t>
+          <t>Resistencias Letradas</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Ana María Ferreira</t>
-        </is>
-      </c>
-      <c r="C309" t="inlineStr"/>
+          <t>Ana María Ferreira Hernández</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new book: El peligro de la historia by Chimamanda Ngozi Adichie in Nini's library
</commit_message>
<xml_diff>
--- a/data/nini/Biblioteca.xlsx
+++ b/data/nini/Biblioteca.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C309"/>
+  <dimension ref="A1:C310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5604,11 +5604,20 @@
           <t>Ana María Ferreira Hernández</t>
         </is>
       </c>
-      <c r="C309" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="C309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>El peligro de la historia</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Chimamanda Ngozi Adichie</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>